<commit_message>
working parameter filtering with all except for hypo, need dat info bb
</commit_message>
<xml_diff>
--- a/Backend/app/datasets/suggestions.xlsx
+++ b/Backend/app/datasets/suggestions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-39860" yWindow="-28800" windowWidth="51200" windowHeight="28800" tabRatio="964" activeTab="1"/>
+    <workbookView xWindow="-39860" yWindow="-28800" windowWidth="51200" windowHeight="28800" tabRatio="964" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MDI advice Before Planned Ex" sheetId="1" r:id="rId1"/>
@@ -4936,7 +4936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C46" sqref="C46:D46"/>
     </sheetView>
   </sheetViews>
@@ -5278,8 +5278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M58" sqref="M58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added new excel sheet
</commit_message>
<xml_diff>
--- a/Backend/app/datasets/suggestions.xlsx
+++ b/Backend/app/datasets/suggestions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Desktop/Projects/GlassByte/Diabetes/Backend/app/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\amnch.ie\dfsroot\Users\finn9m01\Research Diabetes and PA\App project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-39860" yWindow="-28800" windowWidth="51200" windowHeight="28800" tabRatio="964" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="964" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="MDI advice Before Planned Ex" sheetId="1" r:id="rId1"/>
@@ -22,11 +22,8 @@
     <sheet name="Pump Advice After Unplanned Ex" sheetId="8" r:id="rId8"/>
     <sheet name="Links To Advice" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1631,27 +1628,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="118" workbookViewId="0">
       <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" customWidth="1"/>
-    <col min="6" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="57.28515625" customWidth="1"/>
+    <col min="6" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1670,7 +1667,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1687,7 +1684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="D4" s="5" t="s">
         <v>200</v>
@@ -1696,18 +1693,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="E5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E6" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1724,7 +1721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="s">
         <v>200</v>
       </c>
@@ -1732,18 +1729,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="E9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E10" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -1760,7 +1757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>200</v>
       </c>
@@ -1768,13 +1765,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="E13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
@@ -1782,7 +1779,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -1796,17 +1793,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E17" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1830,7 +1827,7 @@
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1847,7 +1844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D21" s="5" t="s">
         <v>200</v>
       </c>
@@ -1855,17 +1852,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E23" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -1882,7 +1879,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D25" s="5" t="s">
         <v>200</v>
       </c>
@@ -1890,17 +1887,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E27" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1912,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
@@ -1930,8 +1927,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:1024" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:1024" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>1</v>
       </c>
@@ -1948,7 +1945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>30</v>
       </c>
@@ -1965,7 +1962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="D35" s="10" t="s">
         <v>200</v>
       </c>
@@ -1973,17 +1970,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
         <v>201</v>
       </c>
@@ -1991,7 +1988,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="s">
         <v>202</v>
       </c>
@@ -1999,7 +1996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>30</v>
       </c>
@@ -2013,18 +2010,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E42" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:1024" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1024" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>30</v>
       </c>
@@ -2041,7 +2038,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="D46" s="10" t="s">
         <v>200</v>
       </c>
@@ -2049,7 +2046,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
         <v>37</v>
       </c>
@@ -4763,12 +4760,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D49" s="5" t="s">
         <v>201</v>
       </c>
@@ -4776,7 +4773,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D50" s="17" t="s">
         <v>202</v>
       </c>
@@ -4784,10 +4781,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="11"/>
     </row>
-    <row r="52" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>30</v>
       </c>
@@ -4802,7 +4799,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>30</v>
       </c>
@@ -4817,9 +4814,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
         <v>1</v>
       </c>
@@ -4836,7 +4833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>39</v>
       </c>
@@ -4851,7 +4848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>39</v>
       </c>
@@ -4866,13 +4863,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E59" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>39</v>
       </c>
@@ -4887,7 +4884,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>39</v>
       </c>
@@ -4902,7 +4899,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="26"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
@@ -4910,14 +4907,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E65" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="27" t="s">
         <v>206</v>
       </c>
@@ -4936,25 +4933,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46:D46"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4985,7 +4982,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
@@ -4999,7 +4996,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -5007,13 +5004,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="D5" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>6</v>
       </c>
@@ -5027,26 +5024,26 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="D7" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="D8" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="D9" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -5077,7 +5074,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>30</v>
       </c>
@@ -5091,7 +5088,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -5099,7 +5096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -5107,13 +5104,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -5144,7 +5141,7 @@
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
     </row>
-    <row r="20" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -5158,12 +5155,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>196</v>
@@ -5172,7 +5169,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -5180,7 +5177,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -5188,13 +5185,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
@@ -5209,12 +5206,12 @@
       </c>
       <c r="F26" s="33"/>
     </row>
-    <row r="27" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>197</v>
@@ -5223,23 +5220,23 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
       <c r="D28" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D29" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5263,7 +5260,7 @@
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>206</v>
       </c>
@@ -5278,26 +5275,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.5" customWidth="1"/>
-    <col min="5" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5316,7 +5313,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -5332,12 +5329,12 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D5" s="5" t="s">
         <v>203</v>
       </c>
@@ -5345,7 +5342,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="16" t="s">
         <v>68</v>
       </c>
@@ -5353,7 +5350,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -5367,17 +5364,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
         <v>204</v>
       </c>
@@ -5385,7 +5382,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D11" s="16" t="s">
         <v>68</v>
       </c>
@@ -5393,7 +5390,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5417,7 +5414,7 @@
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>6</v>
       </c>
@@ -5432,12 +5429,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
         <v>203</v>
       </c>
@@ -5445,7 +5442,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="16" t="s">
         <v>68</v>
       </c>
@@ -5453,7 +5450,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>6</v>
       </c>
@@ -5480,7 +5477,7 @@
       <c r="P18" s="18"/>
       <c r="Q18" s="18"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
         <v>6</v>
       </c>
@@ -5495,7 +5492,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -5514,7 +5511,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -5541,7 +5538,7 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:24" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>30</v>
       </c>
@@ -5563,7 +5560,7 @@
       <c r="W24" s="18"/>
       <c r="X24" s="18"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>78</v>
       </c>
@@ -5575,7 +5572,7 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -5586,7 +5583,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -5597,7 +5594,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:24" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="17" t="s">
         <v>201</v>
       </c>
@@ -5605,7 +5602,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:24" s="7" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="16" t="s">
         <v>202</v>
       </c>
@@ -5613,7 +5610,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
@@ -5627,17 +5624,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -5648,7 +5645,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -5659,8 +5656,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>30</v>
       </c>
@@ -5675,12 +5672,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -5691,7 +5688,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -5702,7 +5699,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D41" s="5" t="s">
         <v>201</v>
       </c>
@@ -5710,7 +5707,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D42" s="17" t="s">
         <v>202</v>
       </c>
@@ -5718,7 +5715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>30</v>
       </c>
@@ -5733,7 +5730,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
@@ -5748,7 +5745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -5767,7 +5764,7 @@
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="21"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -5786,7 +5783,7 @@
       <c r="P46" s="21"/>
       <c r="Q46" s="21"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>1</v>
       </c>
@@ -5813,7 +5810,7 @@
       <c r="P47" s="23"/>
       <c r="Q47" s="23"/>
     </row>
-    <row r="48" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>39</v>
       </c>
@@ -5828,12 +5825,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C49" t="s">
         <v>196</v>
@@ -5842,12 +5839,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E50" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D51" s="17" t="s">
         <v>204</v>
       </c>
@@ -5855,7 +5852,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D52" s="17" t="s">
         <v>68</v>
       </c>
@@ -5863,8 +5860,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:17" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:17" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="35" t="s">
         <v>39</v>
       </c>
@@ -5880,12 +5877,12 @@
       </c>
       <c r="G54" s="33"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>197</v>
@@ -5895,7 +5892,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="26"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -5903,12 +5900,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -5919,7 +5916,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
@@ -5930,7 +5927,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -5949,7 +5946,7 @@
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="27" t="s">
         <v>206</v>
       </c>
@@ -5959,7 +5956,7 @@
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
     </row>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5970,19 +5967,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>86</v>
       </c>
@@ -6024,7 +6021,7 @@
       <c r="AK1" s="11"/>
       <c r="AL1" s="11"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
@@ -6072,7 +6069,7 @@
       <c r="AK2" s="11"/>
       <c r="AL2" s="11"/>
     </row>
-    <row r="3" spans="1:38" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
@@ -6120,7 +6117,7 @@
       <c r="AK3" s="11"/>
       <c r="AL3" s="11"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -6162,7 +6159,7 @@
       <c r="AK4" s="11"/>
       <c r="AL4" s="11"/>
     </row>
-    <row r="5" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -6204,7 +6201,7 @@
       <c r="AK5" s="14"/>
       <c r="AL5" s="14"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>6</v>
       </c>
@@ -6218,22 +6215,22 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="D7" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="D8" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D9" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="43"/>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
@@ -6273,7 +6270,7 @@
       <c r="AK10" s="43"/>
       <c r="AL10" s="43"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -6313,7 +6310,7 @@
       <c r="AK11" s="11"/>
       <c r="AL11" s="11"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
         <v>1</v>
       </c>
@@ -6361,7 +6358,7 @@
       <c r="AK12" s="11"/>
       <c r="AL12" s="11"/>
     </row>
-    <row r="13" spans="1:38" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>30</v>
       </c>
@@ -6409,7 +6406,7 @@
       <c r="AK13" s="11"/>
       <c r="AL13" s="11"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -6451,7 +6448,7 @@
       <c r="AK14" s="11"/>
       <c r="AL14" s="11"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -6493,7 +6490,7 @@
       <c r="AK15" s="11"/>
       <c r="AL15" s="11"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -6535,7 +6532,7 @@
       <c r="AK16" s="11"/>
       <c r="AL16" s="11"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -6575,7 +6572,7 @@
       <c r="AK17" s="11"/>
       <c r="AL17" s="11"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>1</v>
       </c>
@@ -6623,7 +6620,7 @@
       <c r="AK18" s="11"/>
       <c r="AL18" s="11"/>
     </row>
-    <row r="19" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
@@ -6637,12 +6634,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>196</v>
@@ -6685,7 +6682,7 @@
       <c r="AK20" s="11"/>
       <c r="AL20" s="11"/>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -6727,7 +6724,7 @@
       <c r="AK21" s="11"/>
       <c r="AL21" s="11"/>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -6769,7 +6766,7 @@
       <c r="AK22" s="11"/>
       <c r="AL22" s="11"/>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -6811,7 +6808,7 @@
       <c r="AK23" s="11"/>
       <c r="AL23" s="11"/>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -6851,7 +6848,7 @@
       <c r="AK24" s="14"/>
       <c r="AL24" s="14"/>
     </row>
-    <row r="25" spans="1:38" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
         <v>39</v>
       </c>
@@ -6866,12 +6863,12 @@
       </c>
       <c r="F25" s="33"/>
     </row>
-    <row r="26" spans="1:38" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>197</v>
@@ -6914,7 +6911,7 @@
       <c r="AK26" s="11"/>
       <c r="AL26" s="11"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="15"/>
@@ -6956,7 +6953,7 @@
       <c r="AK27" s="11"/>
       <c r="AL27" s="11"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -6998,7 +6995,7 @@
       <c r="AK28" s="11"/>
       <c r="AL28" s="11"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -7040,7 +7037,7 @@
       <c r="AK29" s="11"/>
       <c r="AL29" s="11"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="43"/>
       <c r="B30" s="43"/>
       <c r="C30" s="43"/>
@@ -7080,7 +7077,7 @@
       <c r="AK30" s="11"/>
       <c r="AL30" s="11"/>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>206</v>
       </c>
@@ -7095,25 +7092,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" customWidth="1"/>
-    <col min="5" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" customWidth="1"/>
+    <col min="5" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7132,7 +7129,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -7149,7 +7146,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" s="10" t="s">
         <v>200</v>
       </c>
@@ -7157,17 +7154,17 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E6" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -7184,7 +7181,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="10" t="s">
         <v>200</v>
       </c>
@@ -7192,17 +7189,17 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E10" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -7219,7 +7216,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" s="10" t="s">
         <v>200</v>
       </c>
@@ -7227,17 +7224,17 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E14" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -7251,18 +7248,18 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E17" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>6</v>
       </c>
@@ -7279,7 +7276,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -7290,12 +7287,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -7304,7 +7301,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -7321,7 +7318,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -7332,7 +7329,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>104</v>
       </c>
@@ -7340,7 +7337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -7349,7 +7346,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="18" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" s="18" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>6</v>
       </c>
@@ -7364,7 +7361,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
@@ -7379,31 +7376,31 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="45"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
     </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="43"/>
       <c r="C31" s="43"/>
       <c r="D31" s="43"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
     </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
         <v>1</v>
       </c>
@@ -7420,7 +7417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>30</v>
       </c>
@@ -7438,7 +7435,7 @@
       </c>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -7449,7 +7446,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -7458,7 +7455,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -7467,7 +7464,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -7478,7 +7475,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="7" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -7489,7 +7486,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
         <v>30</v>
       </c>
@@ -7504,7 +7501,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
@@ -7512,7 +7509,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -7521,7 +7518,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -7532,7 +7529,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -7543,19 +7540,19 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="43"/>
       <c r="B46" s="43"/>
       <c r="C46" s="43"/>
       <c r="D46" s="43"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
         <v>30</v>
       </c>
@@ -7572,7 +7569,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -7583,12 +7580,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -7597,7 +7594,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -7608,7 +7605,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="7" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -7619,7 +7616,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="35" t="s">
         <v>30</v>
       </c>
@@ -7634,7 +7631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="35" t="s">
         <v>30</v>
       </c>
@@ -7649,18 +7646,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
       <c r="C56" s="45"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
     </row>
-    <row r="57" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="43"/>
       <c r="C57" s="43"/>
       <c r="D57" s="43"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="39"/>
       <c r="B58" s="39"/>
       <c r="C58" s="39"/>
@@ -7677,7 +7674,7 @@
       <c r="N58" s="21"/>
       <c r="O58" s="21"/>
     </row>
-    <row r="59" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="42" t="s">
         <v>1</v>
       </c>
@@ -7694,7 +7691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>39</v>
       </c>
@@ -7709,12 +7706,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="35" t="s">
         <v>39</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>196</v>
@@ -7724,7 +7721,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
@@ -7733,7 +7730,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -7742,13 +7739,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
     </row>
-    <row r="65" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>39</v>
       </c>
@@ -7764,12 +7761,12 @@
       </c>
       <c r="F65" s="39"/>
     </row>
-    <row r="66" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="35" t="s">
         <v>39</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>197</v>
@@ -7779,7 +7776,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="46"/>
       <c r="B67" s="11"/>
       <c r="C67" s="15"/>
@@ -7788,7 +7785,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="11"/>
       <c r="C68" s="11"/>
@@ -7797,7 +7794,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -7806,19 +7803,19 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="43"/>
       <c r="B70" s="43"/>
       <c r="C70" s="43"/>
       <c r="D70" s="43"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
         <v>206</v>
       </c>
@@ -7835,27 +7832,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView zoomScale="165" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A4" zoomScale="165" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>118</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7886,7 +7883,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
@@ -7900,7 +7897,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -7908,17 +7905,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D5" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
@@ -7932,23 +7929,23 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D8" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D9" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D10" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -7979,139 +7976,125 @@
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+    <row r="14" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B14" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C14" s="15" t="s">
         <v>198</v>
       </c>
+      <c r="D14" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="D18" t="s">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="48" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="18" spans="1:21" s="48" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-    </row>
-    <row r="22" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+    </row>
+    <row r="21" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B21" s="25" t="s">
         <v>7</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="D22" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>198</v>
-      </c>
+      <c r="D22" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="D26" t="s">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+    <row r="27" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
         <v>206</v>
       </c>
     </row>
@@ -8125,26 +8108,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="5" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>127</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8178,7 +8161,7 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -8193,7 +8176,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="9"/>
       <c r="C4" s="11"/>
@@ -8202,12 +8185,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D6" s="5" t="s">
         <v>203</v>
       </c>
@@ -8215,7 +8198,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="16" t="s">
         <v>68</v>
       </c>
@@ -8223,7 +8206,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -8242,12 +8225,12 @@
       <c r="T9" s="44"/>
       <c r="U9" s="44"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -8258,7 +8241,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -8290,8 +8273,8 @@
       <c r="AC12" s="21"/>
       <c r="AD12" s="21"/>
     </row>
-    <row r="13" spans="1:30" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>6</v>
       </c>
@@ -8306,7 +8289,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -8315,12 +8298,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D18" s="5" t="s">
         <v>66</v>
       </c>
@@ -8328,7 +8311,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="16" t="s">
         <v>68</v>
       </c>
@@ -8336,8 +8319,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:22" s="18" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:22" s="18" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
         <v>6</v>
       </c>
@@ -8352,7 +8335,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -8384,7 +8367,7 @@
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
         <v>30</v>
       </c>
@@ -8399,7 +8382,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="35"/>
       <c r="B25" s="15"/>
       <c r="C25" s="11"/>
@@ -8408,7 +8391,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -8419,7 +8402,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -8430,7 +8413,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -8439,7 +8422,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -8450,7 +8433,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -8461,7 +8444,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
         <v>30</v>
       </c>
@@ -8476,7 +8459,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -8484,7 +8467,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -8493,7 +8476,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -8504,7 +8487,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -8515,7 +8498,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -8526,7 +8509,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -8537,7 +8520,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="43"/>
       <c r="B38" s="43"/>
       <c r="C38" s="43"/>
@@ -8578,13 +8561,13 @@
       <c r="AL38" s="3"/>
       <c r="AM38" s="3"/>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>30</v>
       </c>
@@ -8599,12 +8582,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -8613,7 +8596,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -8624,7 +8607,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -8635,7 +8618,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -8646,7 +8629,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:39" s="7" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -8657,7 +8640,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:39" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="49" t="s">
         <v>30</v>
       </c>
@@ -8706,7 +8689,7 @@
       <c r="AL47" s="7"/>
       <c r="AM47" s="7"/>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
         <v>30</v>
       </c>
@@ -8721,7 +8704,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="7"/>
       <c r="C49" s="45"/>
@@ -8762,7 +8745,7 @@
       <c r="AL49" s="7"/>
       <c r="AM49" s="7"/>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
@@ -8794,7 +8777,7 @@
       <c r="U50" s="3"/>
       <c r="V50" s="3"/>
     </row>
-    <row r="51" spans="1:39" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:39" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>39</v>
       </c>
@@ -8808,12 +8791,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:39" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="35" t="s">
         <v>39</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>196</v>
@@ -8823,7 +8806,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -8832,7 +8815,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -8841,7 +8824,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D55" s="5" t="s">
         <v>204</v>
       </c>
@@ -8849,7 +8832,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D56" s="17" t="s">
         <v>68</v>
       </c>
@@ -8857,13 +8840,13 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:39" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
     </row>
-    <row r="58" spans="1:39" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:39" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>39</v>
       </c>
@@ -8877,12 +8860,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:39" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:39" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="35" t="s">
         <v>39</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>197</v>
@@ -8892,7 +8875,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A60" s="46"/>
       <c r="B60" s="11"/>
       <c r="C60" s="15"/>
@@ -8901,7 +8884,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
@@ -8910,7 +8893,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
@@ -8919,7 +8902,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D63" s="5" t="s">
         <v>204</v>
       </c>
@@ -8927,7 +8910,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D64" s="17" t="s">
         <v>68</v>
       </c>
@@ -8935,13 +8918,13 @@
         <v>162</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="43"/>
       <c r="B65" s="43"/>
       <c r="C65" s="43"/>
       <c r="D65" s="43"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
         <v>206</v>
       </c>
@@ -8958,27 +8941,27 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -9009,7 +8992,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
@@ -9023,7 +9006,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -9031,17 +9014,17 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D5" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
@@ -9055,22 +9038,22 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D8" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D9" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D10" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -9093,7 +9076,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -9124,7 +9107,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>30</v>
       </c>
@@ -9138,7 +9121,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -9146,7 +9129,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -9154,12 +9137,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -9183,7 +9166,7 @@
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -9214,67 +9197,81 @@
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
     </row>
-    <row r="21" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
+    <row r="21" spans="1:22" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>57</v>
+      <c r="B21" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="D24" t="s">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
         <v>206</v>
       </c>
     </row>
@@ -9292,13 +9289,13 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>167</v>
       </c>
@@ -9306,22 +9303,22 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="51" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
         <v>172</v>
       </c>
@@ -9329,17 +9326,17 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="51" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
         <v>175</v>
       </c>
@@ -9347,12 +9344,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="50" t="s">
         <v>178</v>
       </c>
@@ -9360,22 +9357,22 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
         <v>183</v>
       </c>
@@ -9383,12 +9380,12 @@
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
         <v>185</v>
       </c>
@@ -9396,17 +9393,17 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="50" t="s">
         <v>189</v>
       </c>
@@ -9414,17 +9411,17 @@
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>104</v>
       </c>

</xml_diff>